<commit_message>
Updated for 3/6 meeting
</commit_message>
<xml_diff>
--- a/Economic Analysis/Extruder Component Costing.xlsx
+++ b/Economic Analysis/Extruder Component Costing.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
   <si>
     <t>Item Name</t>
   </si>
@@ -38,6 +38,9 @@
     <t>Link</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>PET Bottle Recycler</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
     <t>PET Bottle Recycler - Filament Extruder - Free filament - Filament Maker | eBay</t>
   </si>
   <si>
+    <t>Ordered</t>
+  </si>
+  <si>
     <t>EX6 and MDPE10 extruder screws</t>
   </si>
   <si>
@@ -63,6 +69,9 @@
   </si>
   <si>
     <t>https://www.filabot.com/products/ex6-extruder-screws</t>
+  </si>
+  <si>
+    <t>Arrived</t>
   </si>
   <si>
     <t>EX6 EXTRUDER NOZZLES - STYLE X</t>
@@ -84,6 +93,9 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/6771K16/</t>
+  </si>
+  <si>
+    <t>Waiting To Order</t>
   </si>
   <si>
     <t>Single Output Plug-in Shaft for 3/4" Diameter Flexible-Mount Right-Angle Speed Reducer</t>
@@ -187,7 +199,7 @@
     <t>Temperature Coils</t>
   </si>
   <si>
-    <t>temperature Sensors</t>
+    <t>Temperature Sensors</t>
   </si>
   <si>
     <t>Temperature Controllers</t>
@@ -202,28 +214,49 @@
     <t>Screw</t>
   </si>
   <si>
+    <t>All electronics should be 110V</t>
+  </si>
+  <si>
     <t>Nozzle</t>
+  </si>
+  <si>
+    <t>Variable Frequency Drive to control the motor speed</t>
   </si>
   <si>
     <t>Nozzle Plate</t>
   </si>
   <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>PID controller should come with thermistor(?)</t>
+  </si>
+  <si>
     <t>Barrel Flange</t>
+  </si>
+  <si>
+    <t>Give them barrel measurfement with tolerance only on the plus side (size + 0.002 inch)</t>
   </si>
   <si>
     <t>Hopper</t>
   </si>
   <si>
+    <t>length plus or minus 0.0625 inch</t>
+  </si>
+  <si>
     <t>Hopper Barrel Mount</t>
+  </si>
+  <si>
+    <t>explain to them that we are trying or balance cost and hardness of material</t>
   </si>
   <si>
     <t>Enclosure</t>
   </si>
   <si>
-    <t>Fans</t>
+    <t>Draw an arrow and say weldment</t>
   </si>
   <si>
-    <t>Fan Control</t>
+    <t>Fans</t>
   </si>
   <si>
     <t>Motor</t>
@@ -241,13 +274,25 @@
     <t>Recycled PET Pellets</t>
   </si>
   <si>
+    <t>Manufacture ourselves</t>
+  </si>
+  <si>
+    <t>"how hard can you guys make it"</t>
+  </si>
+  <si>
     <t>New PET Pellets</t>
+  </si>
+  <si>
+    <t>Not necessary?</t>
   </si>
   <si>
     <t>Speed Controller Knob</t>
   </si>
   <si>
     <t>Flanged Bearing for Barrel Stability</t>
+  </si>
+  <si>
+    <t>Get Later</t>
   </si>
   <si>
     <t>Barrel Stabilizing Stands</t>
@@ -270,7 +315,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -325,8 +370,14 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +388,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE599"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+        <bgColor rgb="FFEA9999"/>
       </patternFill>
     </fill>
   </fills>
@@ -419,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -442,6 +511,9 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -450,6 +522,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
@@ -467,6 +542,9 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -526,6 +604,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -752,6 +836,7 @@
     <col customWidth="1" min="2" max="2" width="18.13"/>
     <col customWidth="1" min="3" max="3" width="16.5"/>
     <col customWidth="1" min="7" max="7" width="14.5"/>
+    <col customWidth="1" min="9" max="9" width="15.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -779,7 +864,9 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -800,13 +887,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="5">
         <v>286.0</v>
@@ -819,12 +906,14 @@
         <v>286</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -845,31 +934,33 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>869.0</v>
       </c>
       <c r="E3" s="4">
         <v>1.0</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="10">
         <f t="shared" si="1"/>
         <v>869</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>16</v>
+      <c r="H3" s="11" t="s">
+        <v>18</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -889,32 +980,34 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
-        <v>17</v>
+      <c r="A4" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>18</v>
+      <c r="C4" s="14" t="s">
+        <v>21</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="15">
         <v>72.37</v>
       </c>
       <c r="E4" s="4">
         <v>1.0</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="10">
         <f t="shared" si="1"/>
         <v>72.37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -934,32 +1027,34 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="15" t="s">
-        <v>20</v>
+      <c r="A5" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>22</v>
+      <c r="C5" s="17" t="s">
+        <v>25</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="9">
         <v>326.18</v>
       </c>
       <c r="E5" s="4">
         <v>1.0</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="10">
         <f t="shared" si="1"/>
         <v>326.18</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
-      <c r="H5" s="16" t="s">
-        <v>23</v>
+      <c r="H5" s="18" t="s">
+        <v>26</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -979,32 +1074,34 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>21</v>
+      <c r="C6" s="17" t="s">
+        <v>29</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="D6" s="9">
         <v>41.45</v>
       </c>
       <c r="E6" s="4">
         <v>1.0</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="10">
         <f t="shared" si="1"/>
         <v>41.45</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>26</v>
+      <c r="H6" s="11" t="s">
+        <v>30</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -1025,31 +1122,33 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>28</v>
+      <c r="C7" s="17" t="s">
+        <v>32</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>514.0</v>
       </c>
       <c r="E7" s="4">
         <v>1.0</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="10">
         <f t="shared" si="1"/>
         <v>514</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>29</v>
+      <c r="H7" s="11" t="s">
+        <v>33</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -1069,32 +1168,34 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="s">
-        <v>30</v>
+      <c r="A8" s="17" t="s">
+        <v>34</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>31</v>
+      <c r="B8" s="20" t="s">
+        <v>35</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>32</v>
+      <c r="C8" s="21" t="s">
+        <v>36</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="22">
         <v>39.99</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="20">
         <v>3.0</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="23">
         <f t="shared" si="1"/>
         <v>119.97</v>
       </c>
-      <c r="G8" s="17" t="s">
-        <v>11</v>
+      <c r="G8" s="20" t="s">
+        <v>12</v>
       </c>
-      <c r="H8" s="21" t="s">
-        <v>33</v>
+      <c r="H8" s="24" t="s">
+        <v>37</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -1114,32 +1215,34 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="s">
-        <v>34</v>
+      <c r="A9" s="17" t="s">
+        <v>38</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>21</v>
+      <c r="B9" s="20" t="s">
+        <v>24</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>35</v>
+      <c r="C9" s="25" t="s">
+        <v>39</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="26">
         <v>27.49</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="20">
         <v>1.0</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="23">
         <f t="shared" si="1"/>
         <v>27.49</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>11</v>
+      <c r="G9" s="20" t="s">
+        <v>12</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>36</v>
+      <c r="H9" s="11" t="s">
+        <v>40</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1159,32 +1262,34 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="15" t="s">
-        <v>37</v>
+      <c r="A10" s="17" t="s">
+        <v>41</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>21</v>
+      <c r="B10" s="20" t="s">
+        <v>24</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>38</v>
+      <c r="C10" s="27" t="s">
+        <v>42</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="26">
         <v>27.17</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="20">
         <v>2.0</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="23">
         <f t="shared" si="1"/>
         <v>54.34</v>
       </c>
-      <c r="G10" s="17" t="s">
-        <v>11</v>
+      <c r="G10" s="20" t="s">
+        <v>12</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>36</v>
+      <c r="H10" s="11" t="s">
+        <v>40</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1204,32 +1309,34 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11">
-      <c r="A11" s="15" t="s">
-        <v>39</v>
+      <c r="A11" s="17" t="s">
+        <v>43</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>21</v>
+      <c r="B11" s="20" t="s">
+        <v>24</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>40</v>
+      <c r="C11" s="28" t="s">
+        <v>44</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="15">
         <v>35.2</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="20">
         <v>1.0</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="23">
         <f t="shared" si="1"/>
         <v>35.2</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>11</v>
+      <c r="G11" s="20" t="s">
+        <v>12</v>
       </c>
-      <c r="H11" s="21" t="s">
-        <v>41</v>
+      <c r="H11" s="24" t="s">
+        <v>45</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1249,32 +1356,34 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12">
-      <c r="A12" s="26" t="s">
-        <v>42</v>
+      <c r="A12" s="29" t="s">
+        <v>46</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>14</v>
+      <c r="B12" s="20" t="s">
+        <v>16</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>43</v>
+      <c r="C12" s="14" t="s">
+        <v>47</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="15">
         <v>56.27</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="20">
         <v>1.0</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="23">
         <f t="shared" si="1"/>
         <v>56.27</v>
       </c>
-      <c r="G12" s="17" t="s">
-        <v>11</v>
+      <c r="G12" s="20" t="s">
+        <v>19</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>44</v>
+      <c r="H12" s="16" t="s">
+        <v>48</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1294,14 +1403,14 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1322,14 +1431,14 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1350,14 +1459,14 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1378,14 +1487,14 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1406,14 +1515,14 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1434,14 +1543,14 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1462,14 +1571,14 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1490,14 +1599,14 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1518,14 +1627,14 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="31"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1546,14 +1655,14 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="31"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1574,19 +1683,19 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="29" t="s">
-        <v>45</v>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="32" t="s">
+        <v>49</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="33">
         <f>SUM(F2:F22)</f>
         <v>2402.27</v>
       </c>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="31"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1607,14 +1716,14 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="28"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1635,14 +1744,14 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="28"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1663,14 +1772,14 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="28"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1691,14 +1800,14 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="31"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -1719,14 +1828,14 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -1747,14 +1856,14 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="31"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1775,14 +1884,14 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1803,14 +1912,14 @@
       <c r="Z30" s="3"/>
     </row>
     <row r="31">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="31"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -1838,7 +1947,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="28"/>
+      <c r="H32" s="31"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -1866,7 +1975,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="28"/>
+      <c r="H33" s="31"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -28997,285 +29106,332 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="31" t="s">
-        <v>46</v>
+      <c r="A1" s="34" t="s">
+        <v>50</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2">
-      <c r="A2" s="34" t="b">
+      <c r="A2" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>47</v>
+      <c r="B2" s="38" t="s">
+        <v>51</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
     </row>
     <row r="3">
-      <c r="A3" s="38" t="b">
+      <c r="A3" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>48</v>
+      <c r="B3" s="42" t="s">
+        <v>52</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4">
-      <c r="A4" s="34" t="b">
+      <c r="A4" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="39" t="s">
-        <v>49</v>
+      <c r="B4" s="42" t="s">
+        <v>53</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
     </row>
     <row r="5">
-      <c r="A5" s="34" t="b">
+      <c r="A5" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>50</v>
+      <c r="B5" s="42" t="s">
+        <v>54</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6">
-      <c r="A6" s="38" t="b">
+      <c r="A6" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="B6" s="39" t="s">
-        <v>51</v>
+      <c r="B6" s="42" t="s">
+        <v>55</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="7">
-      <c r="A7" s="38" t="b">
+      <c r="A7" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="B7" s="39" t="s">
-        <v>52</v>
+      <c r="B8" s="42" t="s">
+        <v>57</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="37"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="38" t="b">
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="H8" s="43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="B8" s="39" t="s">
-        <v>53</v>
+      <c r="B9" s="42" t="s">
+        <v>59</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="37"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="38" t="b">
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="H9" s="43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>54</v>
+      <c r="B10" s="44" t="s">
+        <v>61</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="34" t="b">
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="39" t="s">
-        <v>55</v>
+      <c r="B15" s="42" t="s">
+        <v>72</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="34" t="b">
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>56</v>
+      <c r="B22" s="42" t="s">
+        <v>82</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="37"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="34" t="b">
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="39" t="s">
-        <v>57</v>
+      <c r="B23" s="42" t="s">
+        <v>83</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="34" t="b">
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="B13" s="39" t="s">
-        <v>58</v>
+      <c r="B25" s="42" t="s">
+        <v>86</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="37"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="34" t="b">
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="B14" s="39" t="s">
-        <v>59</v>
+      <c r="B26" s="42" t="s">
+        <v>87</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="37"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="34" t="b">
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="37" t="b">
         <v>0</v>
       </c>
-      <c r="B15" s="39" t="s">
-        <v>60</v>
+      <c r="B27" s="42" t="s">
+        <v>88</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="37"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="37"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="37"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="37"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="37"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="37"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="37"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="37"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="27">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -29290,20 +29446,19 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>